<commit_message>
Fix ordre virement (carte_sejour,cin) condition issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,19 +429,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>233/DR1</v>
+        <v>908/LF/DIRECTION REGIONALE SUD</v>
       </c>
       <c r="B2" t="str">
-        <v>Direction régionale</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C2" t="str">
-        <v>H354534</v>
+        <v>354646</v>
       </c>
       <c r="D2" t="str">
-        <v xml:space="preserve">VAVA FAFA </v>
+        <v>AGENCE KHATABI</v>
       </c>
       <c r="E2" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F2" t="str">
         <v>mensuelle</v>
@@ -450,13 +450,13 @@
         <v>10</v>
       </c>
       <c r="H2">
-        <v>5000</v>
+        <v>8000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -467,63 +467,392 @@
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>0</v>
+      <c r="N2" t="str">
+        <v>--</v>
       </c>
       <c r="O2">
-        <v>4500</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>908/LF/DIRECTION REGIONALE SUD</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C3" t="str">
+        <v>B12346</v>
+      </c>
+      <c r="D3" t="str">
+        <v>BAKKALI MOHAMED</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>6000</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>600</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="str">
+        <v>--</v>
+      </c>
+      <c r="O3">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>908/LF/DIRECTION REGIONALE SUD</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C4" t="str">
+        <v>L234567</v>
+      </c>
+      <c r="D4" t="str">
+        <v>NACER YASSINE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>2000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="str">
+        <v>--</v>
+      </c>
+      <c r="O4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>389/AOURIR</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C5" t="str">
+        <v>BJ36877</v>
+      </c>
+      <c r="D5" t="str">
+        <v>CHARIJI ABDELLAH</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>7000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>700</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="str">
+        <v>--</v>
+      </c>
+      <c r="O5">
+        <v>6300</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>908/DIRECTION REGIONALE SUD</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C6" t="str">
+        <v>J207703</v>
+      </c>
+      <c r="D6" t="str">
+        <v>ACHENGLI LAILA</v>
+      </c>
+      <c r="E6" t="str">
+        <v>non</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>20000</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>3000</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" t="str">
+        <v>--</v>
+      </c>
+      <c r="O6">
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>900/PATIO</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Siège</v>
+      </c>
+      <c r="C7" t="str">
+        <v>J207703</v>
+      </c>
+      <c r="D7" t="str">
+        <v>ACHENGLI LAILA</v>
+      </c>
+      <c r="E7" t="str">
+        <v>non</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>4500</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>450</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="str">
+        <v>--</v>
+      </c>
+      <c r="O7">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>001/SUP SUD</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Supervision</v>
+      </c>
+      <c r="C8" t="str">
+        <v>354646</v>
+      </c>
+      <c r="D8" t="str">
+        <v>AGENCE KHATABI</v>
+      </c>
+      <c r="E8" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>2400</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="str">
+        <v>--</v>
+      </c>
+      <c r="O8">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>805/KOUTOUBIA</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C9" t="str">
+        <v>L234567</v>
+      </c>
+      <c r="D9" t="str">
+        <v>NACER YASSINE</v>
+      </c>
+      <c r="E9" t="str">
+        <v>non</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9">
+        <v>12000</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>1800</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
+        <v>--</v>
+      </c>
+      <c r="O9">
+        <v>10200</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B3" t="str">
+      <c r="B10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C3" t="str">
+      <c r="C10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D3" t="str">
+      <c r="D10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E3" t="str">
+      <c r="E10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F3" t="str">
+      <c r="F10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G3" t="str">
+      <c r="G10" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H3">
-        <v>5000</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>500</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>4500</v>
+      <c r="H10">
+        <v>61900</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>7350</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>54550</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O10"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove numero compte bancaire unique validation
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,22 +429,22 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
+        <v>389/AOURIR</v>
       </c>
       <c r="B2" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C2" t="str">
-        <v>354646</v>
+        <v>L234567</v>
       </c>
       <c r="D2" t="str">
-        <v>AGENCE KHATABI</v>
+        <v>NACER YASSINE</v>
       </c>
       <c r="E2" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F2" t="str">
-        <v>mensuelle</v>
+        <v>trimestrielle</v>
       </c>
       <c r="G2">
         <v>10</v>
@@ -476,34 +476,34 @@
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B3" t="str">
-        <v>Logement de fonction</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" t="str">
-        <v>B12346</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D3" t="str">
-        <v>BAKKALI MOHAMED</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E3" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H3">
-        <v>6000</v>
+        <v>8000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>600</v>
+        <v>800</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -514,345 +514,16 @@
       <c r="M3">
         <v>0</v>
       </c>
-      <c r="N3" t="str">
-        <v>--</v>
+      <c r="N3">
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>908/LF/DIRECTION REGIONALE SUD</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Logement de fonction</v>
-      </c>
-      <c r="C4" t="str">
-        <v>L234567</v>
-      </c>
-      <c r="D4" t="str">
-        <v>NACER YASSINE</v>
-      </c>
-      <c r="E4" t="str">
-        <v>non</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>2000</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="str">
-        <v>--</v>
-      </c>
-      <c r="O4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>389/AOURIR</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C5" t="str">
-        <v>BJ36877</v>
-      </c>
-      <c r="D5" t="str">
-        <v>CHARIJI ABDELLAH</v>
-      </c>
-      <c r="E5" t="str">
-        <v>non</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>7000</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>700</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="str">
-        <v>--</v>
-      </c>
-      <c r="O5">
-        <v>6300</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>908/DIRECTION REGIONALE SUD</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C6" t="str">
-        <v>J207703</v>
-      </c>
-      <c r="D6" t="str">
-        <v>ACHENGLI LAILA</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>15</v>
-      </c>
-      <c r="H6">
-        <v>20000</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>3000</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="str">
-        <v>--</v>
-      </c>
-      <c r="O6">
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>900/PATIO</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Siège</v>
-      </c>
-      <c r="C7" t="str">
-        <v>J207703</v>
-      </c>
-      <c r="D7" t="str">
-        <v>ACHENGLI LAILA</v>
-      </c>
-      <c r="E7" t="str">
-        <v>non</v>
-      </c>
-      <c r="F7" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7">
-        <v>4500</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>450</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="str">
-        <v>--</v>
-      </c>
-      <c r="O7">
-        <v>4050</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>001/SUP SUD</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Supervision</v>
-      </c>
-      <c r="C8" t="str">
-        <v>354646</v>
-      </c>
-      <c r="D8" t="str">
-        <v>AGENCE KHATABI</v>
-      </c>
-      <c r="E8" t="str">
-        <v>oui</v>
-      </c>
-      <c r="F8" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>2400</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="str">
-        <v>--</v>
-      </c>
-      <c r="O8">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>805/KOUTOUBIA</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Point de vente</v>
-      </c>
-      <c r="C9" t="str">
-        <v>L234567</v>
-      </c>
-      <c r="D9" t="str">
-        <v>NACER YASSINE</v>
-      </c>
-      <c r="E9" t="str">
-        <v>non</v>
-      </c>
-      <c r="F9" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G9">
-        <v>15</v>
-      </c>
-      <c r="H9">
-        <v>12000</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-      <c r="J9">
-        <v>1800</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="str">
-        <v>--</v>
-      </c>
-      <c r="O9">
-        <v>10200</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G10" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H10">
-        <v>61900</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="J10">
-        <v>7350</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10">
-        <v>54550</v>
+        <v>7200</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIx état des taxes pdf issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,101 +429,900 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>389/AOURIR</v>
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
       </c>
       <c r="B2" t="str">
-        <v>Point de vente</v>
+        <v>Logement de fonction</v>
       </c>
       <c r="C2" t="str">
-        <v>L234567</v>
+        <v/>
       </c>
       <c r="D2" t="str">
-        <v>NACER YASSINE</v>
+        <v>NASIRI HASNAA</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
       </c>
       <c r="F2" t="str">
-        <v>trimestrielle</v>
+        <v>mensuelle</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2">
-        <v>8000</v>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>800</v>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>6666.66</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>666.66</v>
       </c>
       <c r="N2" t="str">
         <v>--</v>
       </c>
       <c r="O2">
-        <v>7200</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C3" t="str">
+        <v/>
+      </c>
+      <c r="D3" t="str">
+        <v>BENNIS YOUSRA</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>6666.66</v>
+      </c>
+      <c r="M3">
+        <v>666.66</v>
+      </c>
+      <c r="N3" t="str">
+        <v>--</v>
+      </c>
+      <c r="O3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C4" t="str">
+        <v>CIN605</v>
+      </c>
+      <c r="D4" t="str">
+        <v>SOFIA BADRANE</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4" t="str">
+        <v>--</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>--</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>6666.66</v>
+      </c>
+      <c r="M4">
+        <v>666.66</v>
+      </c>
+      <c r="N4" t="str">
+        <v>--</v>
+      </c>
+      <c r="O4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C5" t="str">
+        <v/>
+      </c>
+      <c r="D5" t="str">
+        <v>NASIRI HASNAA</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
+        <v>3333.33</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>333.33</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>3333.33</v>
+      </c>
+      <c r="O5">
+        <v>6333.33</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C6" t="str">
+        <v/>
+      </c>
+      <c r="D6" t="str">
+        <v>BENNIS YOUSRA</v>
+      </c>
+      <c r="E6" t="str">
+        <v>non</v>
+      </c>
+      <c r="F6" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>3333.33</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>333.33</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>3333.33</v>
+      </c>
+      <c r="O6">
+        <v>6333.33</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Logement de fonction</v>
+      </c>
+      <c r="C7" t="str">
+        <v>CIN605</v>
+      </c>
+      <c r="D7" t="str">
+        <v>SOFIA BADRANE</v>
+      </c>
+      <c r="E7" t="str">
+        <v>non</v>
+      </c>
+      <c r="F7" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>3333.33</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>333.33</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>3333.33</v>
+      </c>
+      <c r="O7">
+        <v>6333.33</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C8" t="str">
+        <v>I83603</v>
+      </c>
+      <c r="D8" t="str">
+        <v>MOHAMED BADRANE</v>
+      </c>
+      <c r="E8" t="str">
+        <v>non</v>
+      </c>
+      <c r="F8" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>446.42</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="str">
+        <v>--</v>
+      </c>
+      <c r="O8">
+        <v>446.42</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C9" t="str">
+        <v>B219321</v>
+      </c>
+      <c r="D9" t="str">
+        <v>JEMAA HORMI</v>
+      </c>
+      <c r="E9" t="str">
+        <v>non</v>
+      </c>
+      <c r="F9" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>1250</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="str">
+        <v>--</v>
+      </c>
+      <c r="O9">
+        <v>1250</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C10" t="str">
+        <v>BK646476</v>
+      </c>
+      <c r="D10" t="str">
+        <v>DOUNIA LAMKADDAM</v>
+      </c>
+      <c r="E10" t="str">
+        <v>non</v>
+      </c>
+      <c r="F10" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>937.5</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="str">
+        <v>--</v>
+      </c>
+      <c r="O10">
+        <v>937.5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C11" t="str">
+        <v>CIN605</v>
+      </c>
+      <c r="D11" t="str">
+        <v>SOFIA BADRANE</v>
+      </c>
+      <c r="E11" t="str">
+        <v>non</v>
+      </c>
+      <c r="F11" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>3750</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>375</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11" t="str">
+        <v>--</v>
+      </c>
+      <c r="O11">
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C12" t="str">
+        <v>I150156</v>
+      </c>
+      <c r="D12" t="str">
+        <v>LATIFA BADRANE</v>
+      </c>
+      <c r="E12" t="str">
+        <v>non</v>
+      </c>
+      <c r="F12" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>223.21</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" t="str">
+        <v>--</v>
+      </c>
+      <c r="O12">
+        <v>223.21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C13" t="str">
+        <v>B171710</v>
+      </c>
+      <c r="D13" t="str">
+        <v>NADIA BADRANE</v>
+      </c>
+      <c r="E13" t="str">
+        <v>non</v>
+      </c>
+      <c r="F13" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>223.21</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13" t="str">
+        <v>--</v>
+      </c>
+      <c r="O13">
+        <v>223.21</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Q194939</v>
+      </c>
+      <c r="D14" t="str">
+        <v>OUAFA BADRANE</v>
+      </c>
+      <c r="E14" t="str">
+        <v>non</v>
+      </c>
+      <c r="F14" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>223.21</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14" t="str">
+        <v>--</v>
+      </c>
+      <c r="O14">
+        <v>223.21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>605/KHOURIBGA NAHDA</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C15" t="str">
+        <v>I210578</v>
+      </c>
+      <c r="D15" t="str">
+        <v>SAID BADRANE</v>
+      </c>
+      <c r="E15" t="str">
+        <v>non</v>
+      </c>
+      <c r="F15" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>446.45</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15" t="str">
+        <v>--</v>
+      </c>
+      <c r="O15">
+        <v>446.45</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>052/FKIH BEN SALEH</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C16" t="str">
+        <v>IB19558</v>
+      </c>
+      <c r="D16" t="str">
+        <v>ZERNAKH ABDELLAH</v>
+      </c>
+      <c r="E16" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F16" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>11000</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16" t="str">
+        <v>--</v>
+      </c>
+      <c r="O16">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>052/FKIH BEN SALEH</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Point de vente</v>
+      </c>
+      <c r="C17" t="str">
+        <v>IB43905</v>
+      </c>
+      <c r="D17" t="str">
+        <v>NHILA BELGACEM</v>
+      </c>
+      <c r="E17" t="str">
+        <v>oui</v>
+      </c>
+      <c r="F17" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17" t="str">
+        <v>--</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C18" t="str">
+        <v>Q251990</v>
+      </c>
+      <c r="D18" t="str">
+        <v>NOUBAIL MOUNTASSIR</v>
+      </c>
+      <c r="E18" t="str">
+        <v>non</v>
+      </c>
+      <c r="F18" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G18">
+        <v>10</v>
+      </c>
+      <c r="H18">
+        <v>6750</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>675</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18" t="str">
+        <v>--</v>
+      </c>
+      <c r="O18">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C19" t="str">
+        <v>IR801997</v>
+      </c>
+      <c r="D19" t="str">
+        <v>NOUBAIL MOHAMMED</v>
+      </c>
+      <c r="E19" t="str">
+        <v>non</v>
+      </c>
+      <c r="F19" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G19">
+        <v>10</v>
+      </c>
+      <c r="H19">
+        <v>6750</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>675</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19" t="str">
+        <v>--</v>
+      </c>
+      <c r="O19">
+        <v>6075</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B3" t="str">
+      <c r="B20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C3" t="str">
+      <c r="C20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D3" t="str">
+      <c r="D20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E3" t="str">
+      <c r="E20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F3" t="str">
+      <c r="F20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G3" t="str">
+      <c r="G20" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H3">
-        <v>8000</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>800</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>7200</v>
+      <c r="H20">
+        <v>41999.99</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>2724.99</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>19999.98</v>
+      </c>
+      <c r="M20">
+        <v>1999.98</v>
+      </c>
+      <c r="N20">
+        <v>9999.99</v>
+      </c>
+      <c r="O20">
+        <v>67274.99</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O20"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Rappel AV cloture issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -449,29 +449,29 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" t="str">
-        <v>--</v>
+      <c r="H2">
+        <v>3333.33</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2" t="str">
-        <v>--</v>
+      <c r="J2">
+        <v>333.33</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>6666.66</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>666.66</v>
+        <v>0</v>
       </c>
       <c r="N2" t="str">
         <v>--</v>
       </c>
       <c r="O2">
-        <v>6000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="3">
@@ -496,29 +496,29 @@
       <c r="G3">
         <v>10</v>
       </c>
-      <c r="H3" t="str">
-        <v>--</v>
+      <c r="H3">
+        <v>3333.33</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
-      <c r="J3" t="str">
-        <v>--</v>
+      <c r="J3">
+        <v>333.33</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>6666.66</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>666.66</v>
+        <v>0</v>
       </c>
       <c r="N3" t="str">
         <v>--</v>
       </c>
       <c r="O3">
-        <v>6000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="4">
@@ -543,108 +543,108 @@
       <c r="G4">
         <v>10</v>
       </c>
-      <c r="H4" t="str">
-        <v>--</v>
+      <c r="H4">
+        <v>3333.33</v>
       </c>
       <c r="I4">
         <v>0</v>
       </c>
-      <c r="J4" t="str">
-        <v>--</v>
+      <c r="J4">
+        <v>333.33</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>6666.66</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>666.66</v>
+        <v>0</v>
       </c>
       <c r="N4" t="str">
         <v>--</v>
       </c>
       <c r="O4">
-        <v>6000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+        <v>052/FKIH BEN SALEH/AV1</v>
       </c>
       <c r="B5" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C5" t="str">
-        <v/>
+        <v>IB19558</v>
       </c>
       <c r="D5" t="str">
-        <v>NASIRI HASNAA</v>
+        <v>ZERNAKH ABDELLAH</v>
       </c>
       <c r="E5" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F5" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>3333.33</v>
+        <v>0</v>
+      </c>
+      <c r="H5" t="str">
+        <v>--</v>
       </c>
       <c r="I5">
         <v>0</v>
       </c>
-      <c r="J5">
-        <v>333.33</v>
+      <c r="J5" t="str">
+        <v>--</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>3333.33</v>
+        <v>450</v>
+      </c>
+      <c r="N5" t="str">
+        <v>--</v>
       </c>
       <c r="O5">
-        <v>6333.33</v>
+        <v>2550</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+        <v>052/FKIH BEN SALEH/AV1</v>
       </c>
       <c r="B6" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C6" t="str">
-        <v/>
+        <v>IB19558</v>
       </c>
       <c r="D6" t="str">
-        <v>BENNIS YOUSRA</v>
+        <v>ZERNAKH ABDELLAH</v>
       </c>
       <c r="E6" t="str">
-        <v>non</v>
+        <v>oui</v>
       </c>
       <c r="F6" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>3333.33</v>
+        <v>12000</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>333.33</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>0</v>
@@ -655,25 +655,25 @@
       <c r="M6">
         <v>0</v>
       </c>
-      <c r="N6">
-        <v>3333.33</v>
+      <c r="N6" t="str">
+        <v>--</v>
       </c>
       <c r="O6">
-        <v>6333.33</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>905/LF/TADLA OUARDIGHA ZAYANE</v>
+        <v>605/KHOURIBGA NAHDA</v>
       </c>
       <c r="B7" t="str">
-        <v>Logement de fonction</v>
+        <v>Point de vente</v>
       </c>
       <c r="C7" t="str">
-        <v>CIN605</v>
+        <v>I83603</v>
       </c>
       <c r="D7" t="str">
-        <v>SOFIA BADRANE</v>
+        <v>MOHAMED BADRANE</v>
       </c>
       <c r="E7" t="str">
         <v>non</v>
@@ -682,16 +682,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>3333.33</v>
+        <v>446.42</v>
       </c>
       <c r="I7">
         <v>0</v>
       </c>
       <c r="J7">
-        <v>333.33</v>
+        <v>0</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -702,11 +702,11 @@
       <c r="M7">
         <v>0</v>
       </c>
-      <c r="N7">
-        <v>3333.33</v>
+      <c r="N7" t="str">
+        <v>--</v>
       </c>
       <c r="O7">
-        <v>6333.33</v>
+        <v>446.42</v>
       </c>
     </row>
     <row r="8">
@@ -717,10 +717,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C8" t="str">
-        <v>I83603</v>
+        <v>B219321</v>
       </c>
       <c r="D8" t="str">
-        <v>MOHAMED BADRANE</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E8" t="str">
         <v>non</v>
@@ -732,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>446.42</v>
+        <v>1250</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -753,7 +753,7 @@
         <v>--</v>
       </c>
       <c r="O8">
-        <v>446.42</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="9">
@@ -764,10 +764,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C9" t="str">
-        <v>B219321</v>
+        <v>BK646476</v>
       </c>
       <c r="D9" t="str">
-        <v>JEMAA HORMI</v>
+        <v>DOUNIA LAMKADDAM</v>
       </c>
       <c r="E9" t="str">
         <v>non</v>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>1250</v>
+        <v>937.5</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -800,7 +800,7 @@
         <v>--</v>
       </c>
       <c r="O9">
-        <v>1250</v>
+        <v>937.5</v>
       </c>
     </row>
     <row r="10">
@@ -811,10 +811,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C10" t="str">
-        <v>BK646476</v>
+        <v>CIN605</v>
       </c>
       <c r="D10" t="str">
-        <v>DOUNIA LAMKADDAM</v>
+        <v>SOFIA BADRANE</v>
       </c>
       <c r="E10" t="str">
         <v>non</v>
@@ -823,16 +823,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H10">
-        <v>937.5</v>
+        <v>3750</v>
       </c>
       <c r="I10">
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -847,7 +847,7 @@
         <v>--</v>
       </c>
       <c r="O10">
-        <v>937.5</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="11">
@@ -858,10 +858,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C11" t="str">
-        <v>CIN605</v>
+        <v>I150156</v>
       </c>
       <c r="D11" t="str">
-        <v>SOFIA BADRANE</v>
+        <v>LATIFA BADRANE</v>
       </c>
       <c r="E11" t="str">
         <v>non</v>
@@ -870,16 +870,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G11">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>3750</v>
+        <v>223.21</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>0</v>
@@ -894,7 +894,7 @@
         <v>--</v>
       </c>
       <c r="O11">
-        <v>3375</v>
+        <v>223.21</v>
       </c>
     </row>
     <row r="12">
@@ -905,10 +905,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C12" t="str">
-        <v>I150156</v>
+        <v>B171710</v>
       </c>
       <c r="D12" t="str">
-        <v>LATIFA BADRANE</v>
+        <v>NADIA BADRANE</v>
       </c>
       <c r="E12" t="str">
         <v>non</v>
@@ -952,10 +952,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C13" t="str">
-        <v>B171710</v>
+        <v>Q194939</v>
       </c>
       <c r="D13" t="str">
-        <v>NADIA BADRANE</v>
+        <v>OUAFA BADRANE</v>
       </c>
       <c r="E13" t="str">
         <v>non</v>
@@ -999,10 +999,10 @@
         <v>Point de vente</v>
       </c>
       <c r="C14" t="str">
-        <v>Q194939</v>
+        <v>I210578</v>
       </c>
       <c r="D14" t="str">
-        <v>OUAFA BADRANE</v>
+        <v>SAID BADRANE</v>
       </c>
       <c r="E14" t="str">
         <v>non</v>
@@ -1014,7 +1014,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>223.21</v>
+        <v>446.45</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1035,21 +1035,21 @@
         <v>--</v>
       </c>
       <c r="O14">
-        <v>223.21</v>
+        <v>446.45</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>605/KHOURIBGA NAHDA</v>
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
       </c>
       <c r="B15" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C15" t="str">
-        <v>I210578</v>
+        <v>Q251990</v>
       </c>
       <c r="D15" t="str">
-        <v>SAID BADRANE</v>
+        <v>NOUBAIL MOUNTASSIR</v>
       </c>
       <c r="E15" t="str">
         <v>non</v>
@@ -1058,16 +1058,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H15">
-        <v>446.45</v>
+        <v>6750</v>
       </c>
       <c r="I15">
         <v>0</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="K15">
         <v>0</v>
@@ -1082,39 +1082,39 @@
         <v>--</v>
       </c>
       <c r="O15">
-        <v>446.45</v>
+        <v>6075</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>052/FKIH BEN SALEH</v>
+        <v>905/TADLA OUARDIGHA ZAYANE</v>
       </c>
       <c r="B16" t="str">
-        <v>Point de vente</v>
+        <v>Direction régionale</v>
       </c>
       <c r="C16" t="str">
-        <v>IB19558</v>
+        <v>IR801997</v>
       </c>
       <c r="D16" t="str">
-        <v>ZERNAKH ABDELLAH</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E16" t="str">
-        <v>oui</v>
+        <v>non</v>
       </c>
       <c r="F16" t="str">
         <v>mensuelle</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H16">
-        <v>11000</v>
+        <v>6750</v>
       </c>
       <c r="I16">
         <v>0</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>675</v>
       </c>
       <c r="K16">
         <v>0</v>
@@ -1129,200 +1129,59 @@
         <v>--</v>
       </c>
       <c r="O16">
-        <v>11000</v>
+        <v>6075</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>052/FKIH BEN SALEH</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B17" t="str">
-        <v>Point de vente</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C17" t="str">
-        <v>IB43905</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D17" t="str">
-        <v>NHILA BELGACEM</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E17" t="str">
-        <v>oui</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F17" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G17" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>42999.99</v>
       </c>
       <c r="I17">
         <v>0</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>2724.99</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="M17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="str">
-        <v>--</v>
+        <v>450</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="str">
-        <v>905/TADLA OUARDIGHA ZAYANE</v>
-      </c>
-      <c r="B18" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C18" t="str">
-        <v>Q251990</v>
-      </c>
-      <c r="D18" t="str">
-        <v>NOUBAIL MOUNTASSIR</v>
-      </c>
-      <c r="E18" t="str">
-        <v>non</v>
-      </c>
-      <c r="F18" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18">
-        <v>6750</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>675</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18" t="str">
-        <v>--</v>
-      </c>
-      <c r="O18">
-        <v>6075</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="str">
-        <v>905/TADLA OUARDIGHA ZAYANE</v>
-      </c>
-      <c r="B19" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C19" t="str">
-        <v>IR801997</v>
-      </c>
-      <c r="D19" t="str">
-        <v>NOUBAIL MOHAMMED</v>
-      </c>
-      <c r="E19" t="str">
-        <v>non</v>
-      </c>
-      <c r="F19" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19">
-        <v>6750</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>675</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19" t="str">
-        <v>--</v>
-      </c>
-      <c r="O19">
-        <v>6075</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G20" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H20">
-        <v>41999.99</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-      <c r="J20">
-        <v>2724.99</v>
-      </c>
-      <c r="K20">
-        <v>0</v>
-      </c>
-      <c r="L20">
-        <v>19999.98</v>
-      </c>
-      <c r="M20">
-        <v>1999.98</v>
-      </c>
-      <c r="N20">
-        <v>9999.99</v>
-      </c>
-      <c r="O20">
-        <v>67274.99</v>
+        <v>42825</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O20"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix resiliation with and without caution issues
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>009/TTT/AV1</v>
+        <v>002/TTT</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>IB19558</v>
+        <v>IR801997</v>
       </c>
       <c r="D2" t="str">
-        <v>ZERNAKH ABDELLAH</v>
+        <v>NOUBAIL MOHAMMED</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -447,16 +447,16 @@
         <v>mensuelle</v>
       </c>
       <c r="G2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -468,42 +468,42 @@
         <v>0</v>
       </c>
       <c r="N2">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>4150</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>009/TTT/AV1</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="B3" t="str">
-        <v>Direction régionale</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C3" t="str">
-        <v>IB19558</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D3" t="str">
-        <v>ZERNAKH ABDELLAH</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="E3" t="str">
-        <v>non</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="F3" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G3" t="str">
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H3">
-        <v>3500</v>
+        <v>2000</v>
       </c>
       <c r="I3">
         <v>0</v>
       </c>
       <c r="J3">
-        <v>350</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -515,203 +515,15 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="O3">
-        <v>3150</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>901/CASABLANCA/AV1</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C4" t="str">
-        <v/>
-      </c>
-      <c r="D4" t="str">
-        <v>NASIRI HASNAA</v>
-      </c>
-      <c r="E4" t="str">
-        <v>non</v>
-      </c>
-      <c r="F4" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4">
-        <v>3166.67</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>316.67</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4" t="str">
-        <v>--</v>
-      </c>
-      <c r="O4">
-        <v>2850</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>901/CASABLANCA/AV1</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C5" t="str">
-        <v>CIN605</v>
-      </c>
-      <c r="D5" t="str">
-        <v>SOFIA BADRANE</v>
-      </c>
-      <c r="E5" t="str">
-        <v>non</v>
-      </c>
-      <c r="F5" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>2666.67</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>266.67</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5" t="str">
-        <v>--</v>
-      </c>
-      <c r="O5">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>901/CASABLANCA/AV1</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Direction régionale</v>
-      </c>
-      <c r="C6" t="str">
-        <v>BK646476</v>
-      </c>
-      <c r="D6" t="str">
-        <v>DOUNIA LAMKADDAM</v>
-      </c>
-      <c r="E6" t="str">
-        <v>non</v>
-      </c>
-      <c r="F6" t="str">
-        <v>mensuelle</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6">
-        <v>2666.67</v>
-      </c>
-      <c r="I6">
-        <v>0</v>
-      </c>
-      <c r="J6">
-        <v>266.67</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="str">
-        <v>--</v>
-      </c>
-      <c r="O6">
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="B7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="E7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="F7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G7" t="str">
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H7">
-        <v>15500.01</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>1550.01</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7">
         <v>2000</v>
-      </c>
-      <c r="O7">
-        <v>14950</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix AV rappel issue
</commit_message>
<xml_diff>
--- a/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
+++ b/download/generated situation/état_des_taxes_xlsx/état_des_taxes_11_2022.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -429,16 +429,16 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>002/TTT</v>
+        <v>001/RRR</v>
       </c>
       <c r="B2" t="str">
         <v>Direction régionale</v>
       </c>
       <c r="C2" t="str">
-        <v>IR801997</v>
+        <v>B219321</v>
       </c>
       <c r="D2" t="str">
-        <v>NOUBAIL MOHAMMED</v>
+        <v>JEMAA HORMI</v>
       </c>
       <c r="E2" t="str">
         <v>non</v>
@@ -449,81 +449,222 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>2000</v>
+      <c r="H2" t="str">
+        <v>--</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
-      <c r="J2">
-        <v>0</v>
+      <c r="J2" t="str">
+        <v>--</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>0</v>
+      <c r="N2" t="str">
+        <v>--</v>
       </c>
       <c r="O2">
-        <v>2000</v>
+        <v>6000</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
+        <v>001/RRR</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C3" t="str">
+        <v>IR801997</v>
+      </c>
+      <c r="D3" t="str">
+        <v>NOUBAIL MOHAMMED</v>
+      </c>
+      <c r="E3" t="str">
+        <v>non</v>
+      </c>
+      <c r="F3" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="str">
+        <v>--</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="str">
+        <v>--</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>6000</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="str">
+        <v>--</v>
+      </c>
+      <c r="O3">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>001/RRR</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C4" t="str">
+        <v>B219321</v>
+      </c>
+      <c r="D4" t="str">
+        <v>JEMAA HORMI</v>
+      </c>
+      <c r="E4" t="str">
+        <v>non</v>
+      </c>
+      <c r="F4" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>001/RRR</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Direction régionale</v>
+      </c>
+      <c r="C5" t="str">
+        <v>IR801997</v>
+      </c>
+      <c r="D5" t="str">
+        <v>NOUBAIL MOHAMMED</v>
+      </c>
+      <c r="E5" t="str">
+        <v>non</v>
+      </c>
+      <c r="F5" t="str">
+        <v>mensuelle</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>1000</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="B3" t="str">
+      <c r="B6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C3" t="str">
+      <c r="C6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D3" t="str">
+      <c r="D6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="E3" t="str">
+      <c r="E6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="F3" t="str">
+      <c r="F6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G3" t="str">
+      <c r="G6" t="str">
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H3">
+      <c r="H6">
         <v>2000</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>2000</v>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>12000</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>14000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:O6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>